<commit_message>
Update to version 1
First complete version
</commit_message>
<xml_diff>
--- a/input/NUTS_regions_germany.xlsx
+++ b/input/NUTS_regions_germany.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bbhberatung-my.sharepoint.com/personal/heinrich_boeing_bbh-beratung_de/Documents/Github/udacity-data_analyst-project2-data_wrangling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bbhberatung-my.sharepoint.com/personal/heinrich_boeing_bbh-beratung_de/Documents/Github/udacity-data_analyst-project2-data_wrangling/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3" documentId="8_{9847790D-B483-4F95-9011-80A103ABA44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F1273C9-4543-4A03-97C7-C7BED3F6C3AD}"/>
@@ -491,7 +491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB3C672-5B86-49D9-B0FC-B5D712393E88}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>